<commit_message>
del corn price excel
</commit_message>
<xml_diff>
--- a/report/DeepProcessOprationAndProfit.xlsx
+++ b/report/DeepProcessOprationAndProfit.xlsx
@@ -1881,8 +1881,8 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="1120062080"/>
-        <c:axId val="1120057184"/>
+        <c:axId val="-1519645664"/>
+        <c:axId val="-1519643488"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -2511,11 +2511,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1120053920"/>
-        <c:axId val="1120062624"/>
+        <c:axId val="-1519636960"/>
+        <c:axId val="-1519645120"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1120062080"/>
+        <c:axId val="-1519645664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2555,7 +2555,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1120057184"/>
+        <c:crossAx val="-1519643488"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -2563,7 +2563,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1120057184"/>
+        <c:axId val="-1519643488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2611,12 +2611,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1120062080"/>
+        <c:crossAx val="-1519645664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1120062624"/>
+        <c:axId val="-1519645120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="50"/>
@@ -2651,12 +2651,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1120053920"/>
+        <c:crossAx val="-1519636960"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="1120053920"/>
+        <c:axId val="-1519636960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2666,7 +2666,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1120062624"/>
+        <c:crossAx val="-1519645120"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -3489,8 +3489,8 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="1120064256"/>
-        <c:axId val="1120064800"/>
+        <c:axId val="-1519642944"/>
+        <c:axId val="-1519634240"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -4119,11 +4119,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1120065344"/>
-        <c:axId val="1120057728"/>
+        <c:axId val="-1519639136"/>
+        <c:axId val="-1519636416"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1120064256"/>
+        <c:axId val="-1519642944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4163,7 +4163,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1120064800"/>
+        <c:crossAx val="-1519634240"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -4171,7 +4171,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1120064800"/>
+        <c:axId val="-1519634240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4219,12 +4219,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1120064256"/>
+        <c:crossAx val="-1519642944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1120057728"/>
+        <c:axId val="-1519636416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="50"/>
@@ -4259,12 +4259,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1120065344"/>
+        <c:crossAx val="-1519639136"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:dateAx>
-        <c:axId val="1120065344"/>
+        <c:axId val="-1519639136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4274,7 +4274,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1120057728"/>
+        <c:crossAx val="-1519636416"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
@@ -5724,8 +5724,8 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="1120065888"/>
-        <c:axId val="1120066432"/>
+        <c:axId val="-1519639680"/>
+        <c:axId val="-1519644576"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -6354,11 +6354,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1120051744"/>
-        <c:axId val="1120056096"/>
+        <c:axId val="-1519648928"/>
+        <c:axId val="-1519642400"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1120065888"/>
+        <c:axId val="-1519639680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6398,7 +6398,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1120066432"/>
+        <c:crossAx val="-1519644576"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -6406,7 +6406,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1120066432"/>
+        <c:axId val="-1519644576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6454,12 +6454,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1120065888"/>
+        <c:crossAx val="-1519639680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1120056096"/>
+        <c:axId val="-1519642400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6493,12 +6493,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1120051744"/>
+        <c:crossAx val="-1519648928"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:dateAx>
-        <c:axId val="1120051744"/>
+        <c:axId val="-1519648928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6508,7 +6508,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1120056096"/>
+        <c:crossAx val="-1519642400"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
@@ -7194,8 +7194,8 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="1120052288"/>
-        <c:axId val="857745840"/>
+        <c:axId val="-1519647296"/>
+        <c:axId val="-1519641856"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -7824,11 +7824,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="938207200"/>
-        <c:axId val="857750736"/>
+        <c:axId val="-1519641312"/>
+        <c:axId val="-1519635872"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1120052288"/>
+        <c:axId val="-1519647296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7868,7 +7868,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="857745840"/>
+        <c:crossAx val="-1519641856"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -7876,7 +7876,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="857745840"/>
+        <c:axId val="-1519641856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7924,12 +7924,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1120052288"/>
+        <c:crossAx val="-1519647296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="857750736"/>
+        <c:axId val="-1519635872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7963,12 +7963,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="938207200"/>
+        <c:crossAx val="-1519641312"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:dateAx>
-        <c:axId val="938207200"/>
+        <c:axId val="-1519641312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7978,7 +7978,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="857750736"/>
+        <c:crossAx val="-1519635872"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
@@ -11312,10 +11312,10 @@
   <dimension ref="A1:AH97"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B78" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B84" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="K98" sqref="K98"/>
+      <selection pane="bottomRight" activeCell="A98" sqref="A98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>

</xml_diff>